<commit_message>
Hotels search Test Case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
@@ -3,9 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{81EEC0E3-8A4A-46A3-AB4A-2C6E436625C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahmoud El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AD310C-BBB3-4F7E-A44E-34CCA9FF8A0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="19515" windowHeight="16500" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="testsheet1" sheetId="2" r:id="rId1"/>
@@ -13,7 +18,6 @@
     <sheet name="testsheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:G11"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +27,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>TC ID/Name</t>
+  </si>
+  <si>
+    <t>testingHotelsSearch</t>
+  </si>
+  <si>
+    <t>Destination</t>
+  </si>
+  <si>
+    <t>Checkin Date</t>
+  </si>
+  <si>
+    <t>Checkout Date</t>
+  </si>
+  <si>
+    <t>Grand Plaza Serviced</t>
+  </si>
+  <si>
+    <t>02/02/2021</t>
+  </si>
+  <si>
+    <t>Expected</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -78,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -87,6 +116,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -407,7 +439,7 @@
   <sheetViews>
     <sheetView zoomScale="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -418,26 +450,48 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="A1:C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="10.625" style="1"/>
+    <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.58203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.9140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.58203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D2" s="2"/>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>44197</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
   </sheetData>
@@ -453,7 +507,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Finish Hotels Search test case & Enhancements
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C798EE-AF36-4EC2-A413-CA9BD2B2D194}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6C750D-599C-440A-83CA-DD3AC483B597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="testsheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="testsheet2" sheetId="1" r:id="rId2"/>
+    <sheet name="GUI" sheetId="1" r:id="rId2"/>
     <sheet name="testsheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>TC ID/Name</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Checkin Date</t>
+  </si>
+  <si>
+    <t>Expected Hotel Name</t>
+  </si>
+  <si>
+    <t>Grand Plaza Apartments</t>
   </si>
 </sst>
 </file>
@@ -444,7 +450,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -453,7 +459,7 @@
     <col min="2" max="2" width="18.25" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.625" style="1"/>
+    <col min="5" max="5" width="21.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -469,7 +475,9 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -484,7 +492,9 @@
       <c r="D2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add Hotels Reservation test case for API level
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6C750D-599C-440A-83CA-DD3AC483B597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B93F3FF-3B51-46C8-BD32-F106D486FFAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
-    <sheet name="testsheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="API" sheetId="2" r:id="rId1"/>
     <sheet name="GUI" sheetId="1" r:id="rId2"/>
     <sheet name="testsheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>TC ID/Name</t>
   </si>
@@ -38,22 +38,46 @@
     <t>Destination</t>
   </si>
   <si>
-    <t>Checkout Date</t>
-  </si>
-  <si>
     <t>Grand Plaza Serviced</t>
   </si>
   <si>
     <t>02/02/2021</t>
   </si>
   <si>
-    <t>Checkin Date</t>
-  </si>
-  <si>
     <t>Expected Hotel Name</t>
   </si>
   <si>
     <t>Grand Plaza Apartments</t>
+  </si>
+  <si>
+    <t>City Name</t>
+  </si>
+  <si>
+    <t>Hotel Name</t>
+  </si>
+  <si>
+    <t>Check In Date</t>
+  </si>
+  <si>
+    <t>Check Out Date</t>
+  </si>
+  <si>
+    <t>Adults Count</t>
+  </si>
+  <si>
+    <t>Child Count</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>london</t>
+  </si>
+  <si>
+    <t>grand-plaza-apartments</t>
+  </si>
+  <si>
+    <t>02-02-2021</t>
   </si>
 </sst>
 </file>
@@ -435,12 +459,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A63622E-CB57-6443-8D5E-E59E3D20E8B5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -449,16 +537,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E5A4EB-72C8-0E44-91C4-D3652BB51352}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -470,13 +558,13 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -484,16 +572,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished Reservation Hotels Search test case
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
+++ b/src/test/resources/TestData/LiveProject_PhpTravels_ReservationHotelsSearch_TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahmoud El-Sharkawy\git\Automation-Practice\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B93F3FF-3B51-46C8-BD32-F106D486FFAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F4F7113-DF4D-4065-86B0-61025337ACC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{26E33DF7-E585-0646-A302-1C346031F2A4}"/>
   </bookViews>
   <sheets>
     <sheet name="API" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>TC ID/Name</t>
   </si>
@@ -461,22 +461,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A63622E-CB57-6443-8D5E-E59E3D20E8B5}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.58203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -502,7 +502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -535,22 +535,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2E5A4EB-72C8-0E44-91C4-D3652BB51352}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.25" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.9140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.4140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.4140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.08203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -564,10 +567,16 @@
         <v>10</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -580,7 +589,13 @@
       <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1">
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -597,7 +612,7 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.58203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>